<commit_message>
add custom shape criterias
</commit_message>
<xml_diff>
--- a/tables/configTable_monthly.xlsx
+++ b/tables/configTable_monthly.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3074" yWindow="0" windowWidth="21129" windowHeight="9152"/>
+    <workbookView xWindow="4185" yWindow="0" windowWidth="21135" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>line</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,16 +36,6 @@
   <si>
     <t>高牌号硅钢</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高端家电用钢</t>
-  </si>
-  <si>
-    <t>汽车面板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>先进高强汽车用钢</t>
   </si>
   <si>
     <t>grade_col</t>
@@ -399,13 +389,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
@@ -417,13 +407,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -434,122 +424,38 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>2250</v>
+        <v>1580</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>2250</v>
+        <v>1580</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>2250</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>1580</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>1580</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>1580</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>1580</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>1580</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>